<commit_message>
all save and work
</commit_message>
<xml_diff>
--- a/data/answers.xlsx
+++ b/data/answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,28 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Kachanov Aleksandr Igorevich</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Неудовлетворительные</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Не обеспечены</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Не обеспечены</t>
+          <t>Вопросы</t>
         </is>
       </c>
     </row>

</xml_diff>